<commit_message>
Chun's NF Quiz new
</commit_message>
<xml_diff>
--- a/SQL評量_正規化_Chun v1.xlsx
+++ b/SQL評量_正規化_Chun v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\JAVA班\git_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7552B264-0808-4A2B-9172-1C403D7088B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910940A7-AAED-4595-AAC8-C8780797E058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{36CE15E8-7DE5-4D3C-B6E0-1B1AB355C8A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="140">
   <si>
     <r>
       <rPr>
@@ -1755,13 +1755,481 @@
       <t>公寓</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>F011</t>
+  </si>
+  <si>
+    <t>F012</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮中埔街20號</t>
+  </si>
+  <si>
+    <t>100人)</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮和平街79號</t>
+  </si>
+  <si>
+    <t>3142人)</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮龍山路三段142號</t>
+  </si>
+  <si>
+    <t>1072)</t>
+  </si>
+  <si>
+    <t>苗栗縣後龍鎮中華路1498號</t>
+  </si>
+  <si>
+    <t>32)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市米市街80號</t>
+  </si>
+  <si>
+    <t>106人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市光復路117號</t>
+  </si>
+  <si>
+    <t>26人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市博愛街109號</t>
+  </si>
+  <si>
+    <t>2038人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市大同路53號</t>
+  </si>
+  <si>
+    <t>128人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市民族里和平路102號</t>
+  </si>
+  <si>
+    <t>353人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市忠孝忠孝一路69號</t>
+  </si>
+  <si>
+    <t>501人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市信義里中正路65號</t>
+  </si>
+  <si>
+    <t>194人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市信義里中正路116號</t>
+  </si>
+  <si>
+    <t>78人)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>容納人數</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮中埔街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮和平街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>79</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮龍山路三段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>142</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣後龍鎮中華路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1498</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市米市街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市光復路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>117</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市博愛街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市大同路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市民族里和平路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>102</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市忠孝忠孝一路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>69</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市信義里中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>65</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市信義里中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>116</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1802,6 +2270,21 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
     </font>
@@ -1993,12 +2476,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2011,20 +2497,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2071,12 +2545,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -2089,12 +2557,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="千分位" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2406,7 +2905,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1A47CA-532C-4318-8D23-1C0A59A513C2}">
-  <dimension ref="A1:AF25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K11"/>
@@ -2430,37 +2929,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="5" t="s">
         <v>69</v>
       </c>
       <c r="M1" s="1"/>
@@ -2496,16 +2995,16 @@
       <c r="G2" s="1">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M2" s="1"/>
@@ -2541,16 +3040,16 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M3" s="1"/>
@@ -2586,16 +3085,16 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M4" s="1"/>
@@ -2631,16 +3130,16 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M5" s="1"/>
@@ -2676,16 +3175,16 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="M6" s="1"/>
@@ -2721,16 +3220,16 @@
       <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="M7" s="1"/>
@@ -2766,16 +3265,16 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M8" s="1"/>
@@ -2811,16 +3310,16 @@
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M9" s="1"/>
@@ -2856,16 +3355,16 @@
       <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M10" s="1"/>
@@ -2901,16 +3400,16 @@
       <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M11" s="1"/>
@@ -2925,10 +3424,6 @@
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -2988,114 +3483,15 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="13:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-    </row>
+    <row r="17" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="18" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="20" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="22" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="24" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="25" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3107,10 +3503,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:AD13"/>
+  <dimension ref="A1:AB15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3133,682 +3529,745 @@
     <col min="16" max="16" width="8.875" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.625" style="1" customWidth="1"/>
     <col min="18" max="18" width="6.5" style="1" customWidth="1"/>
-    <col min="19" max="19" width="61.375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="6.875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="4.375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="7.75" style="1" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="8" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5" style="1" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="8.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="6.375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="6.75" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="9" style="1"/>
+    <col min="19" max="19" width="32.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="4.375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="7.75" style="1" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="8" style="1" customWidth="1"/>
+    <col min="25" max="25" width="9.5" style="1" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="8.125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="6.375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="6.75" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="26"/>
+      <c r="D1" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="H1" s="7" t="s">
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="H1" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="26"/>
+      <c r="K1" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="O1" s="7" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="O1" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="R1" s="6" t="s">
+      <c r="P1" s="26"/>
+      <c r="R1" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="6" t="s">
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="X1" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="H2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="O2" s="10" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="O2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="10"/>
-      <c r="R2" s="10" t="s">
+      <c r="P2" s="6"/>
+      <c r="R2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:28" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="U3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="W3" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="X3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="Y3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="Z3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AA3" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="AB3" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="S4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T4" s="5">
+      <c r="S4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="T4" s="32">
+        <v>100</v>
+      </c>
+      <c r="U4" s="4">
         <v>1</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="W4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W4" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V4,Final!B:B,Final!A:A)</f>
+      <c r="X4" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W4,Final!B:B,Final!A:A)</f>
         <v>C001</v>
       </c>
-      <c r="X4" s="5" t="s">
+      <c r="Y4" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="Y4" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V4,Q!C2,Q!H2)</f>
+      <c r="Z4" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W4,Q!C2,Q!H2)</f>
         <v>M001</v>
       </c>
-      <c r="Z4" s="5" t="str">
+      <c r="AA4" s="4" t="str">
         <f>R4</f>
         <v>F001</v>
       </c>
-      <c r="AA4" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X4,Final!P:P,Final!O:O)</f>
+      <c r="AB4" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y4,Final!P:P,Final!O:O)</f>
         <v>B001</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="T5" s="5">
+      <c r="S5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="T5" s="32">
+        <v>3142</v>
+      </c>
+      <c r="U5" s="4">
         <v>1</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="W5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="W5" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V5,Final!B:B,Final!A:A)</f>
+      <c r="X5" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W5,Final!B:B,Final!A:A)</f>
         <v>C002</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="Y5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Y5" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V5,Q!C3,Q!H3)</f>
+      <c r="Z5" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W5,Q!C3,Q!H3)</f>
         <v>M001</v>
       </c>
-      <c r="Z5" s="5" t="str">
-        <f t="shared" ref="Z5:Z13" si="0">R5</f>
+      <c r="AA5" s="4" t="str">
+        <f t="shared" ref="AA5:AA13" si="0">R5</f>
         <v>F002</v>
       </c>
-      <c r="AA5" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X5,Final!P:P,Final!O:O)</f>
+      <c r="AB5" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y5,Final!P:P,Final!O:O)</f>
         <v>B002</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="R6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="S6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="T6" s="5">
+      <c r="S6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="T6" s="32">
+        <v>1072</v>
+      </c>
+      <c r="U6" s="4">
         <v>1</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="W6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="W6" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V6,Final!B:B,Final!A:A)</f>
+      <c r="X6" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W6,Final!B:B,Final!A:A)</f>
         <v>C003</v>
       </c>
-      <c r="X6" s="5" t="s">
+      <c r="Y6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Y6" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V6,Q!C4,Q!H4)</f>
+      <c r="Z6" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W6,Q!C4,Q!H4)</f>
         <v>M001</v>
       </c>
-      <c r="Z6" s="5" t="str">
+      <c r="AA6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>F003</v>
       </c>
-      <c r="AA6" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X6,Final!P:P,Final!O:O)</f>
+      <c r="AB6" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y6,Final!P:P,Final!O:O)</f>
         <v>B002</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="T7" s="5">
+      <c r="S7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="T7" s="32">
+        <v>32</v>
+      </c>
+      <c r="U7" s="4">
         <v>1</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="W7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="W7" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V7,Final!B:B,Final!A:A)</f>
+      <c r="X7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W7,Final!B:B,Final!A:A)</f>
         <v>C004</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="Y7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V7,Q!C5,Q!H5)</f>
+      <c r="Z7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W7,Q!C5,Q!H5)</f>
         <v>M001</v>
       </c>
-      <c r="Z7" s="5" t="str">
+      <c r="AA7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>F004</v>
       </c>
-      <c r="AA7" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X7,Final!P:P,Final!O:O)</f>
+      <c r="AB7" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y7,Final!P:P,Final!O:O)</f>
         <v>B003</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="S8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" s="5">
+      <c r="S8" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="T8" s="32">
+        <v>106</v>
+      </c>
+      <c r="U8" s="4">
         <v>1</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="W8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="W8" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V8,Final!B:B,Final!A:A)</f>
+      <c r="X8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W8,Final!B:B,Final!A:A)</f>
         <v>C005</v>
       </c>
-      <c r="X8" s="5" t="s">
+      <c r="Y8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="Y8" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V8,Q!C6,Q!H6)</f>
+      <c r="Z8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W8,Q!C6,Q!H6)</f>
         <v>M002</v>
       </c>
-      <c r="Z8" s="5" t="str">
+      <c r="AA8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>F005</v>
       </c>
-      <c r="AA8" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X8,Final!P:P,Final!O:O)</f>
+      <c r="AB8" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y8,Final!P:P,Final!O:O)</f>
         <v>B001</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="S9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="T9" s="5">
+      <c r="S9" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="T9" s="32">
+        <v>26</v>
+      </c>
+      <c r="U9" s="4">
+        <v>1</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W9,Final!B:B,Final!A:A)</f>
+        <v>C005</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W9,Q!C7,Q!H7)</f>
+        <v>M002</v>
+      </c>
+      <c r="AA9" s="4" t="str">
+        <f>R10</f>
+        <v>F007</v>
+      </c>
+      <c r="AB9" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y9,Final!P:P,Final!O:O)</f>
+        <v>B002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="S10" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="T10" s="32">
+        <v>2038</v>
+      </c>
+      <c r="U10" s="4">
         <v>2</v>
       </c>
-      <c r="V9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="W9" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V9,Final!B:B,Final!A:A)</f>
-        <v>C005</v>
-      </c>
-      <c r="X9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y9" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V9,Q!C7,Q!H7)</f>
-        <v>M002</v>
-      </c>
-      <c r="Z9" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>F006</v>
-      </c>
-      <c r="AA9" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X9,Final!P:P,Final!O:O)</f>
-        <v>B002</v>
+      <c r="W10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="X10" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W10,Final!B:B,Final!A:A)</f>
+        <v>C006</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z10" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W10,Q!C8,Q!H8)</f>
+        <v>M003</v>
+      </c>
+      <c r="AA10" s="4" t="str">
+        <f>R12</f>
+        <v>F009</v>
+      </c>
+      <c r="AB10" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y10,Final!P:P,Final!O:O)</f>
+        <v>B003</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="S11" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="T11" s="32">
+        <v>128</v>
+      </c>
+      <c r="U11" s="4">
+        <v>1</v>
+      </c>
+      <c r="W11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T10" s="5">
+      <c r="X11" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W11,Final!B:B,Final!A:A)</f>
+        <v>C007</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z11" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W11,Q!C9,Q!H9)</f>
+        <v>M003</v>
+      </c>
+      <c r="AA11" s="4" t="str">
+        <f>R13</f>
+        <v>F010</v>
+      </c>
+      <c r="AB11" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y11,Final!P:P,Final!O:O)</f>
+        <v>B004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="S12" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="T12" s="32">
+        <v>353</v>
+      </c>
+      <c r="U12" s="4">
         <v>1</v>
       </c>
-      <c r="V10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="W10" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V10,Final!B:B,Final!A:A)</f>
-        <v>C006</v>
-      </c>
-      <c r="X10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y10" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V10,Q!C8,Q!H8)</f>
+      <c r="W12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X12" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W12,Final!B:B,Final!A:A)</f>
+        <v>C008</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W12,Q!C10,Q!H10)</f>
         <v>M003</v>
       </c>
-      <c r="Z10" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>F007</v>
-      </c>
-      <c r="AA10" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X10,Final!P:P,Final!O:O)</f>
-        <v>B003</v>
+      <c r="AA12" s="4" t="str">
+        <f>R14</f>
+        <v>F011</v>
+      </c>
+      <c r="AB12" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y12,Final!P:P,Final!O:O)</f>
+        <v>B001</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="5" t="s">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="S13" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="T13" s="32">
+        <v>501</v>
+      </c>
+      <c r="U13" s="4">
+        <v>1</v>
+      </c>
+      <c r="W13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T11" s="5">
+      <c r="X13" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W13,Final!B:B,Final!A:A)</f>
+        <v>C008</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z13" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W13,Q!C11,Q!H11)</f>
+        <v>M003</v>
+      </c>
+      <c r="AA13" s="4" t="str">
+        <f>R15</f>
+        <v>F012</v>
+      </c>
+      <c r="AB13" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y13,Final!P:P,Final!O:O)</f>
+        <v>B004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="S14" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="T14" s="32">
+        <v>194</v>
+      </c>
+      <c r="U14" s="4">
         <v>1</v>
       </c>
-      <c r="V11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="W11" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V11,Final!B:B,Final!A:A)</f>
-        <v>C007</v>
-      </c>
-      <c r="X11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y11" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V11,Q!C9,Q!H9)</f>
-        <v>M003</v>
-      </c>
-      <c r="Z11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>F008</v>
-      </c>
-      <c r="AA11" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X11,Final!P:P,Final!O:O)</f>
-        <v>B004</v>
-      </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="R12" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="T12" s="5">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="R15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="S15" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="T15" s="32">
+        <v>78</v>
+      </c>
+      <c r="U15" s="4">
         <v>1</v>
-      </c>
-      <c r="V12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="W12" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V12,Final!B:B,Final!A:A)</f>
-        <v>C008</v>
-      </c>
-      <c r="X12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V12,Q!C10,Q!H10)</f>
-        <v>M003</v>
-      </c>
-      <c r="Z12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>F009</v>
-      </c>
-      <c r="AA12" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X12,Final!P:P,Final!O:O)</f>
-        <v>B001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="R13" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="T13" s="5">
-        <v>1</v>
-      </c>
-      <c r="V13" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="W13" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V13,Final!B:B,Final!A:A)</f>
-        <v>C008</v>
-      </c>
-      <c r="X13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y13" s="5" t="str">
-        <f>_xlfn.XLOOKUP(V13,Q!C11,Q!H11)</f>
-        <v>M003</v>
-      </c>
-      <c r="Z13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>F010</v>
-      </c>
-      <c r="AA13" s="5" t="str">
-        <f>_xlfn.XLOOKUP(X13,Final!P:P,Final!O:O)</f>
-        <v>B004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="X1:AB1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="D1:F1"/>
@@ -3822,10 +4281,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFFB8F4-D09E-4E08-A4DE-C97D3C4FE0DC}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3:AB14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3839,10 +4298,11 @@
     <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26.125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="32.75" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:22" ht="33.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:29" ht="33.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -3855,50 +4315,50 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="5" t="s">
         <v>67</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -3911,22 +4371,22 @@
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="18" t="s">
         <v>2</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -3935,26 +4395,32 @@
       <c r="P3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="R3" s="19">
+      <c r="R3" s="15">
         <v>1</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="S3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="26" t="s">
+      <c r="T3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="27" t="s">
+      <c r="U3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="27" t="s">
+      <c r="V3" s="21" t="s">
         <v>9</v>
       </c>
+      <c r="AB3" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>104</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -3967,22 +4433,22 @@
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="18" t="s">
         <v>12</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -3991,26 +4457,32 @@
       <c r="P4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="Q4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="19">
+      <c r="R4" s="15">
         <v>1</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="26" t="s">
+      <c r="T4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="V4" s="27" t="s">
+      <c r="V4" s="21" t="s">
         <v>9</v>
       </c>
+      <c r="AB4" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -4023,22 +4495,22 @@
       <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="18" t="s">
         <v>17</v>
       </c>
       <c r="O5" s="3" t="s">
@@ -4047,26 +4519,32 @@
       <c r="P5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="19">
+      <c r="R5" s="15">
         <v>1</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="S5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="T5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="U5" s="27" t="s">
+      <c r="U5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="V5" s="27" t="s">
+      <c r="V5" s="21" t="s">
         <v>9</v>
       </c>
+      <c r="AB5" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -4079,13 +4557,13 @@
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="18" t="s">
         <v>23</v>
       </c>
       <c r="O6" s="3" t="s">
@@ -4094,26 +4572,32 @@
       <c r="P6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="19">
+      <c r="R6" s="15">
         <v>1</v>
       </c>
-      <c r="S6" s="24" t="s">
+      <c r="S6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="T6" s="26" t="s">
+      <c r="T6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="27" t="s">
+      <c r="U6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="27" t="s">
+      <c r="V6" s="21" t="s">
         <v>9</v>
       </c>
+      <c r="AB6" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -4126,13 +4610,13 @@
       <c r="D7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="M7" s="18" t="s">
+      <c r="M7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="22" t="s">
+      <c r="N7" s="18" t="s">
         <v>28</v>
       </c>
       <c r="O7" s="3" t="s">
@@ -4141,26 +4625,32 @@
       <c r="P7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q7" s="29" t="s">
+      <c r="Q7" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="R7" s="19">
+      <c r="R7" s="15">
         <v>1</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="S7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="T7" s="26" t="s">
+      <c r="T7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="27" t="s">
+      <c r="U7" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V7" s="27" t="s">
+      <c r="V7" s="21" t="s">
         <v>35</v>
       </c>
+      <c r="AB7" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -4173,13 +4663,13 @@
       <c r="D8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="N8" s="22" t="s">
+      <c r="N8" s="18" t="s">
         <v>28</v>
       </c>
       <c r="O8" s="3" t="s">
@@ -4188,26 +4678,32 @@
       <c r="P8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="29" t="s">
+      <c r="Q8" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="R8" s="19">
+      <c r="R8" s="15">
         <v>2</v>
       </c>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="T8" s="26" t="s">
+      <c r="T8" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="U8" s="27" t="s">
+      <c r="U8" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="V8" s="27" t="s">
+      <c r="V8" s="21" t="s">
         <v>35</v>
       </c>
+      <c r="AB8" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -4220,13 +4716,13 @@
       <c r="D9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="L9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="22" t="s">
+      <c r="N9" s="18" t="s">
         <v>38</v>
       </c>
       <c r="O9" s="3" t="s">
@@ -4235,33 +4731,39 @@
       <c r="P9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="18" t="s">
+      <c r="Q9" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="R9" s="19">
+      <c r="R9" s="15">
         <v>1</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="S9" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="T9" s="26" t="s">
+      <c r="T9" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U9" s="27" t="s">
+      <c r="U9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="V9" s="27" t="s">
+      <c r="V9" s="21" t="s">
         <v>45</v>
       </c>
+      <c r="AB9" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>116</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="L10" s="14" t="s">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="L10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="22" t="s">
+      <c r="N10" s="18" t="s">
         <v>48</v>
       </c>
       <c r="O10" s="3" t="s">
@@ -4270,33 +4772,39 @@
       <c r="P10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Q10" s="18" t="s">
+      <c r="Q10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10" s="15">
         <v>1</v>
       </c>
-      <c r="S10" s="24" t="s">
+      <c r="S10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="T10" s="26" t="s">
+      <c r="T10" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U10" s="27" t="s">
+      <c r="U10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="V10" s="27" t="s">
+      <c r="V10" s="21" t="s">
         <v>45</v>
       </c>
+      <c r="AB10" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="L11" s="14" t="s">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="L11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M11" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="18" t="s">
         <v>53</v>
       </c>
       <c r="O11" s="3" t="s">
@@ -4305,33 +4813,39 @@
       <c r="P11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="Q11" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="R11" s="19">
+      <c r="R11" s="15">
         <v>1</v>
       </c>
-      <c r="S11" s="24" t="s">
+      <c r="S11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="T11" s="26" t="s">
+      <c r="T11" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="U11" s="27" t="s">
+      <c r="U11" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="V11" s="27" t="s">
+      <c r="V11" s="21" t="s">
         <v>45</v>
       </c>
+      <c r="AB11" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>120</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L12" s="15" t="s">
+    <row r="12" spans="1:29" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="19" t="s">
         <v>53</v>
       </c>
       <c r="O12" s="3" t="s">
@@ -4340,26 +4854,47 @@
       <c r="P12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q12" s="20" t="s">
+      <c r="Q12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="R12" s="21">
+      <c r="R12" s="17">
         <v>1</v>
       </c>
-      <c r="S12" s="25" t="s">
+      <c r="S12" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="T12" s="28" t="s">
+      <c r="T12" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="U12" s="27" t="s">
+      <c r="U12" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="V12" s="27" t="s">
+      <c r="V12" s="21" t="s">
         <v>45</v>
       </c>
+      <c r="AB12" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>122</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:29" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AB13" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AB14" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CHun's NF Quiz updated
</commit_message>
<xml_diff>
--- a/SQL評量_正規化_Chun v1.xlsx
+++ b/SQL評量_正規化_Chun v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\JAVA班\git_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910940A7-AAED-4595-AAC8-C8780797E058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F187BCB-945D-4722-88FB-FD09B3854AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{36CE15E8-7DE5-4D3C-B6E0-1B1AB355C8A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="141">
   <si>
     <r>
       <rPr>
@@ -1576,6 +1576,129 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
+      <t>關於分局的事</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>設施別</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>關於村里設施</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>村里設施、管轄分局總覽</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>村里辦公室地址</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>設施別代號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>設施代號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>地址</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>地下樓層數</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
       <t>村里別</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1583,39 +1706,132 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>關於分局的事</t>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>村里別代號</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>設施別</t>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>設施代號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>公寓</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>關於村里設施</t>
+    <t>F011</t>
+  </si>
+  <si>
+    <t>F012</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮中埔街20號</t>
+  </si>
+  <si>
+    <t>100人)</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮和平街79號</t>
+  </si>
+  <si>
+    <t>3142人)</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮龍山路三段142號</t>
+  </si>
+  <si>
+    <t>1072)</t>
+  </si>
+  <si>
+    <t>苗栗縣後龍鎮中華路1498號</t>
+  </si>
+  <si>
+    <t>32)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市米市街80號</t>
+  </si>
+  <si>
+    <t>106人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市光復路117號</t>
+  </si>
+  <si>
+    <t>26人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市博愛街109號</t>
+  </si>
+  <si>
+    <t>2038人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市大同路53號</t>
+  </si>
+  <si>
+    <t>128人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市民族里和平路102號</t>
+  </si>
+  <si>
+    <t>353人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市忠孝忠孝一路69號</t>
+  </si>
+  <si>
+    <t>501人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市信義里中正路65號</t>
+  </si>
+  <si>
+    <t>194人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市信義里中正路116號</t>
+  </si>
+  <si>
+    <t>78人)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>容納人數</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1628,8 +1844,371 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>村里設施、管轄分局總覽</t>
-    </r>
+      <t>苗栗縣竹南鎮中埔街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮和平街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>79</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮龍山路三段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>142</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣後龍鎮中華路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1498</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市米市街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市光復路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>117</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市博愛街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市大同路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市民族里和平路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>102</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市忠孝忠孝一路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>69</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市信義里中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>65</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市信義里中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>116</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <t>SQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -1638,587 +2217,23 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>村里辦公室地址</t>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>設施</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>類別</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>設施別代號</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>設施代號</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>地址</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>地下樓層數</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>村里別</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>村里別代號</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>設施代號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>公寓</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>F011</t>
-  </si>
-  <si>
-    <t>F012</t>
-  </si>
-  <si>
-    <t>苗栗縣竹南鎮中埔街20號</t>
-  </si>
-  <si>
-    <t>100人)</t>
-  </si>
-  <si>
-    <t>苗栗縣竹南鎮和平街79號</t>
-  </si>
-  <si>
-    <t>3142人)</t>
-  </si>
-  <si>
-    <t>苗栗縣竹南鎮龍山路三段142號</t>
-  </si>
-  <si>
-    <t>1072)</t>
-  </si>
-  <si>
-    <t>苗栗縣後龍鎮中華路1498號</t>
-  </si>
-  <si>
-    <t>32)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市米市街80號</t>
-  </si>
-  <si>
-    <t>106人)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市光復路117號</t>
-  </si>
-  <si>
-    <t>26人)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市博愛街109號</t>
-  </si>
-  <si>
-    <t>2038人)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市大同路53號</t>
-  </si>
-  <si>
-    <t>128人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市民族里和平路102號</t>
-  </si>
-  <si>
-    <t>353人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市忠孝忠孝一路69號</t>
-  </si>
-  <si>
-    <t>501人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市信義里中正路65號</t>
-  </si>
-  <si>
-    <t>194人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市信義里中正路116號</t>
-  </si>
-  <si>
-    <t>78人)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>容納人數</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣竹南鎮中埔街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣竹南鎮和平街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>79</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣竹南鎮龍山路三段</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>142</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣後龍鎮中華路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1498</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市米市街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>80</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市光復路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>117</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市博愛街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>109</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市大同路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>53</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市民族里和平路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>102</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市忠孝忠孝一路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>69</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市信義里中正路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>65</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市信義里中正路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>116</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -2227,9 +2242,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2287,6 +2302,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Microsoft JhengHei"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2484,7 +2506,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2558,6 +2580,24 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2565,30 +2605,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2908,10 +2924,10 @@
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K11"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
@@ -2928,7 +2944,7 @@
     <col min="23" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="34.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>59</v>
       </c>
@@ -2973,7 +2989,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3018,7 +3034,7 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3063,7 +3079,7 @@
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -3108,7 +3124,7 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -3153,7 +3169,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
     </row>
-    <row r="6" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="31.5">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -3198,7 +3214,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="31.5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -3243,7 +3259,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="15.75">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -3288,7 +3304,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="15.75">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
@@ -3333,7 +3349,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="15.75">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -3378,7 +3394,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="15.75">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -3423,7 +3439,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="15.75">
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -3435,7 +3451,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="15.75">
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -3447,7 +3463,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="15.75">
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -3459,7 +3475,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="15.75">
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -3471,7 +3487,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="15.75">
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -3483,15 +3499,15 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="25" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="17" s="1" customFormat="1" ht="15.75"/>
+    <row r="18" s="1" customFormat="1" ht="15.75"/>
+    <row r="19" s="1" customFormat="1" ht="15.75"/>
+    <row r="20" s="1" customFormat="1" ht="15.75"/>
+    <row r="21" s="1" customFormat="1" ht="15.75"/>
+    <row r="22" s="1" customFormat="1" ht="15.75"/>
+    <row r="23" s="1" customFormat="1" ht="15.75"/>
+    <row r="24" s="1" customFormat="1" ht="15.75"/>
+    <row r="25" s="1" customFormat="1" ht="15.75"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3505,11 +3521,11 @@
   </sheetPr>
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="7.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
@@ -3530,56 +3546,54 @@
     <col min="17" max="17" width="4.625" style="1" customWidth="1"/>
     <col min="18" max="18" width="6.5" style="1" customWidth="1"/>
     <col min="19" max="19" width="32.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.25" style="28" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.875" style="1" customWidth="1"/>
     <col min="22" max="22" width="4.375" style="1" customWidth="1"/>
     <col min="23" max="23" width="7.75" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="8" style="1" customWidth="1"/>
+    <col min="24" max="24" width="6.25" style="1" customWidth="1"/>
     <col min="25" max="25" width="9.5" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="8.125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="6.375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="6.75" style="1" customWidth="1"/>
+    <col min="26" max="28" width="6.25" style="1" customWidth="1"/>
     <col min="29" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:28">
+      <c r="A1" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="D1" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="H1" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="32"/>
+      <c r="K1" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="D1" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="H1" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="26"/>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="O1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="32"/>
+      <c r="R1" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="R1" s="24" t="s">
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="X1" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="X1" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" s="6" t="s">
         <v>58</v>
       </c>
@@ -3610,7 +3624,7 @@
         <v>58</v>
       </c>
       <c r="S2" s="6"/>
-      <c r="T2" s="31"/>
+      <c r="T2" s="26"/>
       <c r="U2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
@@ -3619,7 +3633,7 @@
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>60</v>
       </c>
@@ -3630,7 +3644,7 @@
         <v>61</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>63</v>
@@ -3651,28 +3665,28 @@
         <v>69</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>59</v>
       </c>
       <c r="R3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="S3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="T3" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="U3" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="T3" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="U3" s="7" t="s">
+      <c r="W3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="X3" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>98</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>59</v>
@@ -3681,13 +3695,13 @@
         <v>66</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -3728,9 +3742,9 @@
         <v>73</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="T4" s="32">
+        <v>127</v>
+      </c>
+      <c r="T4" s="27">
         <v>100</v>
       </c>
       <c r="U4" s="4">
@@ -3744,10 +3758,10 @@
         <v>C001</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Z4" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W4,Q!C2,Q!H2)</f>
+        <f>_xlfn.XLOOKUP(W4,Q!C:C,Q!H:H)</f>
         <v>M001</v>
       </c>
       <c r="AA4" s="4" t="str">
@@ -3759,7 +3773,7 @@
         <v>B001</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -3800,9 +3814,9 @@
         <v>74</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="T5" s="32">
+        <v>128</v>
+      </c>
+      <c r="T5" s="27">
         <v>3142</v>
       </c>
       <c r="U5" s="4">
@@ -3819,11 +3833,11 @@
         <v>10</v>
       </c>
       <c r="Z5" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W5,Q!C3,Q!H3)</f>
+        <f>_xlfn.XLOOKUP(W5,Q!C:C,Q!H:H)</f>
         <v>M001</v>
       </c>
       <c r="AA5" s="4" t="str">
-        <f t="shared" ref="AA5:AA13" si="0">R5</f>
+        <f t="shared" ref="AA5:AA15" si="0">R5</f>
         <v>F002</v>
       </c>
       <c r="AB5" s="4" t="str">
@@ -3831,7 +3845,7 @@
         <v>B002</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -3872,9 +3886,9 @@
         <v>75</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="T6" s="32">
+        <v>129</v>
+      </c>
+      <c r="T6" s="27">
         <v>1072</v>
       </c>
       <c r="U6" s="4">
@@ -3891,7 +3905,7 @@
         <v>10</v>
       </c>
       <c r="Z6" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W6,Q!C4,Q!H4)</f>
+        <f>_xlfn.XLOOKUP(W6,Q!C:C,Q!H:H)</f>
         <v>M001</v>
       </c>
       <c r="AA6" s="4" t="str">
@@ -3903,7 +3917,7 @@
         <v>B002</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -3929,9 +3943,9 @@
         <v>76</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="T7" s="32">
+        <v>130</v>
+      </c>
+      <c r="T7" s="27">
         <v>32</v>
       </c>
       <c r="U7" s="4">
@@ -3948,7 +3962,7 @@
         <v>21</v>
       </c>
       <c r="Z7" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W7,Q!C5,Q!H5)</f>
+        <f>_xlfn.XLOOKUP(W7,Q!C:C,Q!H:H)</f>
         <v>M001</v>
       </c>
       <c r="AA7" s="4" t="str">
@@ -3960,7 +3974,7 @@
         <v>B003</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -3979,10 +3993,10 @@
       <c r="R8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="S8" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="T8" s="32">
+      <c r="S8" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="T8" s="27">
         <v>106</v>
       </c>
       <c r="U8" s="4">
@@ -3999,7 +4013,7 @@
         <v>0</v>
       </c>
       <c r="Z8" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W8,Q!C6,Q!H6)</f>
+        <f>_xlfn.XLOOKUP(W8,Q!C:C,Q!H:H)</f>
         <v>M002</v>
       </c>
       <c r="AA8" s="4" t="str">
@@ -4011,7 +4025,7 @@
         <v>B001</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28">
       <c r="A9" s="4" t="s">
         <v>37</v>
       </c>
@@ -4030,10 +4044,10 @@
       <c r="R9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="S9" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="T9" s="32">
+      <c r="S9" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="T9" s="27">
         <v>26</v>
       </c>
       <c r="U9" s="4">
@@ -4047,22 +4061,22 @@
         <v>C005</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="Z9" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W9,Q!C7,Q!H7)</f>
+        <f>_xlfn.XLOOKUP(W9,Q!C:C,Q!H:H)</f>
         <v>M002</v>
       </c>
       <c r="AA9" s="4" t="str">
-        <f>R10</f>
-        <v>F007</v>
+        <f t="shared" si="0"/>
+        <v>F006</v>
       </c>
       <c r="AB9" s="4" t="str">
         <f>_xlfn.XLOOKUP(Y9,Final!P:P,Final!O:O)</f>
-        <v>B002</v>
+        <v>B001</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28">
       <c r="A10" s="4" t="s">
         <v>47</v>
       </c>
@@ -4081,39 +4095,39 @@
       <c r="R10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="S10" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="T10" s="32">
+      <c r="S10" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="T10" s="27">
         <v>2038</v>
       </c>
       <c r="U10" s="4">
         <v>2</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="X10" s="4" t="str">
         <f>_xlfn.XLOOKUP(W10,Final!B:B,Final!A:A)</f>
-        <v>C006</v>
+        <v>C005</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="Z10" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W10,Q!C8,Q!H8)</f>
-        <v>M003</v>
+        <f>_xlfn.XLOOKUP(W10,Q!C:C,Q!H:H)</f>
+        <v>M002</v>
       </c>
       <c r="AA10" s="4" t="str">
-        <f>R12</f>
-        <v>F009</v>
+        <f t="shared" si="0"/>
+        <v>F007</v>
       </c>
       <c r="AB10" s="4" t="str">
         <f>_xlfn.XLOOKUP(Y10,Final!P:P,Final!O:O)</f>
-        <v>B003</v>
+        <v>B002</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28">
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
@@ -4132,136 +4146,180 @@
       <c r="R11" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="S11" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="T11" s="32">
+      <c r="S11" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="T11" s="27">
         <v>128</v>
       </c>
       <c r="U11" s="4">
         <v>1</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="X11" s="4" t="str">
         <f>_xlfn.XLOOKUP(W11,Final!B:B,Final!A:A)</f>
-        <v>C007</v>
+        <v>C005</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="Z11" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W11,Q!C9,Q!H9)</f>
-        <v>M003</v>
+        <f>_xlfn.XLOOKUP(W11,Q!C:C,Q!H:H)</f>
+        <v>M002</v>
       </c>
       <c r="AA11" s="4" t="str">
-        <f>R13</f>
-        <v>F010</v>
+        <f t="shared" si="0"/>
+        <v>F008</v>
       </c>
       <c r="AB11" s="4" t="str">
         <f>_xlfn.XLOOKUP(Y11,Final!P:P,Final!O:O)</f>
-        <v>B004</v>
+        <v>B002</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28">
       <c r="R12" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="S12" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="T12" s="32">
+      <c r="S12" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="T12" s="27">
         <v>353</v>
       </c>
       <c r="U12" s="4">
         <v>1</v>
       </c>
       <c r="W12" s="4" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="X12" s="4" t="str">
         <f>_xlfn.XLOOKUP(W12,Final!B:B,Final!A:A)</f>
-        <v>C008</v>
+        <v>C006</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="Z12" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W12,Q!C10,Q!H10)</f>
+        <f>_xlfn.XLOOKUP(W12,Q!C:C,Q!H:H)</f>
         <v>M003</v>
       </c>
       <c r="AA12" s="4" t="str">
-        <f>R14</f>
-        <v>F011</v>
+        <f t="shared" si="0"/>
+        <v>F009</v>
       </c>
       <c r="AB12" s="4" t="str">
         <f>_xlfn.XLOOKUP(Y12,Final!P:P,Final!O:O)</f>
-        <v>B001</v>
+        <v>B003</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28">
       <c r="R13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="S13" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="T13" s="32">
+      <c r="S13" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="T13" s="27">
         <v>501</v>
       </c>
       <c r="U13" s="4">
         <v>1</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="X13" s="4" t="str">
         <f>_xlfn.XLOOKUP(W13,Final!B:B,Final!A:A)</f>
-        <v>C008</v>
+        <v>C007</v>
       </c>
       <c r="Y13" s="4" t="s">
         <v>46</v>
       </c>
       <c r="Z13" s="4" t="str">
-        <f>_xlfn.XLOOKUP(W13,Q!C11,Q!H11)</f>
+        <f>_xlfn.XLOOKUP(W13,Q!C:C,Q!H:H)</f>
         <v>M003</v>
       </c>
       <c r="AA13" s="4" t="str">
-        <f>R15</f>
-        <v>F012</v>
+        <f t="shared" si="0"/>
+        <v>F010</v>
       </c>
       <c r="AB13" s="4" t="str">
         <f>_xlfn.XLOOKUP(Y13,Final!P:P,Final!O:O)</f>
         <v>B004</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28">
       <c r="R14" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="S14" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="T14" s="32">
+        <v>100</v>
+      </c>
+      <c r="S14" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="T14" s="27">
         <v>194</v>
       </c>
       <c r="U14" s="4">
         <v>1</v>
       </c>
+      <c r="W14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X14" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W14,Final!B:B,Final!A:A)</f>
+        <v>C008</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W14,Q!C:C,Q!H:H)</f>
+        <v>M003</v>
+      </c>
+      <c r="AA14" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>F011</v>
+      </c>
+      <c r="AB14" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y14,Final!P:P,Final!O:O)</f>
+        <v>B001</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28">
       <c r="R15" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="S15" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="T15" s="32">
+        <v>101</v>
+      </c>
+      <c r="S15" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="T15" s="27">
         <v>78</v>
       </c>
       <c r="U15" s="4">
         <v>1</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X15" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W15,Final!B:B,Final!A:A)</f>
+        <v>C008</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z15" s="4" t="str">
+        <f>_xlfn.XLOOKUP(W15,Q!C:C,Q!H:H)</f>
+        <v>M003</v>
+      </c>
+      <c r="AA15" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>F012</v>
+      </c>
+      <c r="AB15" s="4" t="str">
+        <f>_xlfn.XLOOKUP(Y15,Final!P:P,Final!O:O)</f>
+        <v>B004</v>
       </c>
     </row>
   </sheetData>
@@ -4287,7 +4345,7 @@
       <selection activeCell="AB3" sqref="AB3:AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="12" max="12" width="9.5" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="7.5" bestFit="1" customWidth="1"/>
@@ -4298,11 +4356,11 @@
     <col min="20" max="20" width="9.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26.125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="32.75" style="28" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="32.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:29" ht="33.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="17.25" thickBot="1"/>
+    <row r="2" spans="1:29" ht="33.75" thickTop="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4358,7 +4416,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -4413,14 +4471,14 @@
       <c r="V3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="29" t="s">
+      <c r="AB3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC3" t="s">
         <v>103</v>
       </c>
-      <c r="AC3" t="s">
-        <v>104</v>
-      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -4475,14 +4533,14 @@
       <c r="V4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AB4" s="29" t="s">
+      <c r="AB4" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AC4" t="s">
         <v>105</v>
       </c>
-      <c r="AC4" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -4537,14 +4595,14 @@
       <c r="V5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AB5" s="29" t="s">
+      <c r="AB5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC5" t="s">
         <v>107</v>
       </c>
-      <c r="AC5" t="s">
-        <v>108</v>
-      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -4590,14 +4648,14 @@
       <c r="V6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AB6" s="29" t="s">
+      <c r="AB6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC6" t="s">
         <v>109</v>
       </c>
-      <c r="AC6" t="s">
-        <v>110</v>
-      </c>
     </row>
-    <row r="7" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" ht="31.5">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -4643,14 +4701,14 @@
       <c r="V7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="AB7" s="30" t="s">
+      <c r="AB7" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC7" t="s">
         <v>111</v>
       </c>
-      <c r="AC7" t="s">
-        <v>112</v>
-      </c>
     </row>
-    <row r="8" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" ht="31.5">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -4696,14 +4754,14 @@
       <c r="V8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="AB8" s="30" t="s">
+      <c r="AB8" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC8" t="s">
         <v>113</v>
       </c>
-      <c r="AC8" t="s">
-        <v>114</v>
-      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -4749,14 +4807,14 @@
       <c r="V9" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AB9" s="30" t="s">
+      <c r="AB9" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC9" t="s">
         <v>115</v>
       </c>
-      <c r="AC9" t="s">
-        <v>116</v>
-      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29">
       <c r="L10" s="10" t="s">
         <v>46</v>
       </c>
@@ -4790,14 +4848,14 @@
       <c r="V10" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AB10" s="30" t="s">
+      <c r="AB10" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC10" t="s">
         <v>117</v>
       </c>
-      <c r="AC10" t="s">
-        <v>118</v>
-      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29">
       <c r="L11" s="10" t="s">
         <v>0</v>
       </c>
@@ -4831,14 +4889,14 @@
       <c r="V11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AB11" s="30" t="s">
+      <c r="AB11" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC11" t="s">
         <v>119</v>
       </c>
-      <c r="AC11" t="s">
-        <v>120</v>
-      </c>
     </row>
-    <row r="12" spans="1:29" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="17.25" thickBot="1">
       <c r="L12" s="11" t="s">
         <v>46</v>
       </c>
@@ -4872,27 +4930,27 @@
       <c r="V12" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AB12" s="30" t="s">
+      <c r="AB12" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC12" t="s">
         <v>121</v>
       </c>
-      <c r="AC12" t="s">
+    </row>
+    <row r="13" spans="1:29" ht="17.25" thickTop="1">
+      <c r="AB13" s="25" t="s">
         <v>122</v>
       </c>
+      <c r="AC13" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="13" spans="1:29" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="AB13" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC13" t="s">
+    <row r="14" spans="1:29">
+      <c r="AB14" s="25" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="AB14" s="30" t="s">
+      <c r="AC14" t="s">
         <v>125</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chun's Quiz 1 SQL
</commit_message>
<xml_diff>
--- a/SQL評量_正規化_Chun v1.xlsx
+++ b/SQL評量_正規化_Chun v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\JAVA班\git_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F187BCB-945D-4722-88FB-FD09B3854AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449CA91F-E3D4-4D18-B46B-C3F216960C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{36CE15E8-7DE5-4D3C-B6E0-1B1AB355C8A4}"/>
   </bookViews>
@@ -1490,32 +1490,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>關於村里的事</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>分局</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>FK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1570,52 +1544,56 @@
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>關於分局的事</t>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>村里辦公室地址</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>設施別</t>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>設施別代號</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>關於村里設施</t>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>設施代號</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>村里設施、管轄分局總覽</t>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>地址</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1629,7 +1607,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>村里辦公室地址</t>
+      <t>地下樓層數</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1643,7 +1621,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>設施別代號</t>
+      <t>村里別</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1657,11 +1635,115 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
+      <t>村里別代號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
       <t>設施代號</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>公寓</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>F011</t>
+  </si>
+  <si>
+    <t>F012</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮中埔街20號</t>
+  </si>
+  <si>
+    <t>100人)</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮和平街79號</t>
+  </si>
+  <si>
+    <t>3142人)</t>
+  </si>
+  <si>
+    <t>苗栗縣竹南鎮龍山路三段142號</t>
+  </si>
+  <si>
+    <t>1072)</t>
+  </si>
+  <si>
+    <t>苗栗縣後龍鎮中華路1498號</t>
+  </si>
+  <si>
+    <t>32)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市米市街80號</t>
+  </si>
+  <si>
+    <t>106人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市光復路117號</t>
+  </si>
+  <si>
+    <t>26人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市博愛街109號</t>
+  </si>
+  <si>
+    <t>2038人)</t>
+  </si>
+  <si>
+    <t>苗栗縣苗栗市大同路53號</t>
+  </si>
+  <si>
+    <t>128人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市民族里和平路102號</t>
+  </si>
+  <si>
+    <t>353人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市忠孝忠孝一路69號</t>
+  </si>
+  <si>
+    <t>501人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市信義里中正路65號</t>
+  </si>
+  <si>
+    <t>194人)</t>
+  </si>
+  <si>
+    <t>苗栗縣頭份市信義里中正路116號</t>
+  </si>
+  <si>
+    <t>78人)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1671,568 +1753,432 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>地址</t>
+      <t>容納人數</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮中埔街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮和平街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>79</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣竹南鎮龍山路三段</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>142</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣後龍鎮中華路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1498</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市米市街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市光復路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>117</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市博愛街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣苗栗市大同路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市民族里和平路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>102</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市忠孝忠孝一路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>69</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市信義里中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>65</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗縣頭份市信義里中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>116</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>地下樓層數</t>
+        <rFont val="Microsoft JhengHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>設施</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>類別</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>村里別</t>
-    </r>
+    <t>SQL_VILLAGE</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>村里別代號</t>
-    </r>
+    <t>VILLAGES</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>設施代號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>公寓</t>
-    </r>
+    <t>SQL_POLICE</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>F011</t>
-  </si>
-  <si>
-    <t>F012</t>
-  </si>
-  <si>
-    <t>苗栗縣竹南鎮中埔街20號</t>
-  </si>
-  <si>
-    <t>100人)</t>
-  </si>
-  <si>
-    <t>苗栗縣竹南鎮和平街79號</t>
-  </si>
-  <si>
-    <t>3142人)</t>
-  </si>
-  <si>
-    <t>苗栗縣竹南鎮龍山路三段142號</t>
-  </si>
-  <si>
-    <t>1072)</t>
-  </si>
-  <si>
-    <t>苗栗縣後龍鎮中華路1498號</t>
-  </si>
-  <si>
-    <t>32)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市米市街80號</t>
-  </si>
-  <si>
-    <t>106人)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市光復路117號</t>
-  </si>
-  <si>
-    <t>26人)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市博愛街109號</t>
-  </si>
-  <si>
-    <t>2038人)</t>
-  </si>
-  <si>
-    <t>苗栗縣苗栗市大同路53號</t>
-  </si>
-  <si>
-    <t>128人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市民族里和平路102號</t>
-  </si>
-  <si>
-    <t>353人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市忠孝忠孝一路69號</t>
-  </si>
-  <si>
-    <t>501人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市信義里中正路65號</t>
-  </si>
-  <si>
-    <t>194人)</t>
-  </si>
-  <si>
-    <t>苗栗縣頭份市信義里中正路116號</t>
-  </si>
-  <si>
-    <t>78人)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>容納人數</t>
-    </r>
+    <t>POLICES</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣竹南鎮中埔街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣竹南鎮和平街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>79</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣竹南鎮龍山路三段</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>142</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣後龍鎮中華路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1498</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市米市街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>80</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市光復路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>117</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市博愛街</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>109</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣苗栗市大同路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>53</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市民族里和平路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>102</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市忠孝忠孝一路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>69</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市信義里中正路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>65</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市信義里中正路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>116</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-  </si>
-  <si>
-    <t>SQ</t>
+    <t>SQL_BUILDING</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Microsoft JhengHei"/>
-        <family val="2"/>
-      </rPr>
-      <t>設施</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>類別</t>
-    </r>
+    <t>FACILITIES</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VILLAGES_INFO</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3521,8 +3467,8 @@
   </sheetPr>
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3558,35 +3504,35 @@
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="31" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B1" s="32"/>
       <c r="D1" s="30" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="H1" s="31" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="I1" s="32"/>
       <c r="K1" s="30" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="O1" s="31" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="P1" s="32"/>
       <c r="R1" s="30" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
       <c r="U1" s="30"/>
       <c r="X1" s="30" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="Y1" s="30"/>
       <c r="Z1" s="30"/>
@@ -3598,10 +3544,10 @@
         <v>58</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -3609,10 +3555,10 @@
         <v>58</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -3644,7 +3590,7 @@
         <v>61</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>63</v>
@@ -3665,28 +3611,28 @@
         <v>69</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>59</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="X3" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="Y3" s="8" t="s">
         <v>59</v>
@@ -3695,10 +3641,10 @@
         <v>66</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -3733,16 +3679,16 @@
         <v>9</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="T4" s="27">
         <v>100</v>
@@ -3758,7 +3704,7 @@
         <v>C001</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="Z4" s="4" t="str">
         <f>_xlfn.XLOOKUP(W4,Q!C:C,Q!H:H)</f>
@@ -3805,16 +3751,16 @@
         <v>35</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="T5" s="27">
         <v>3142</v>
@@ -3877,16 +3823,16 @@
         <v>45</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="T6" s="27">
         <v>1072</v>
@@ -3934,16 +3880,16 @@
         <v>25</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>46</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="T7" s="27">
         <v>32</v>
@@ -3991,10 +3937,10 @@
         <v>30</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S8" s="24" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="T8" s="27">
         <v>106</v>
@@ -4042,10 +3988,10 @@
         <v>40</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="S9" s="24" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="T9" s="27">
         <v>26</v>
@@ -4093,10 +4039,10 @@
         <v>50</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="S10" s="24" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="T10" s="27">
         <v>2038</v>
@@ -4144,10 +4090,10 @@
         <v>55</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S11" s="24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="T11" s="27">
         <v>128</v>
@@ -4180,10 +4126,10 @@
     </row>
     <row r="12" spans="1:28">
       <c r="R12" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="S12" s="24" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="T12" s="27">
         <v>353</v>
@@ -4216,10 +4162,10 @@
     </row>
     <row r="13" spans="1:28">
       <c r="R13" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S13" s="24" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="T13" s="27">
         <v>501</v>
@@ -4252,10 +4198,10 @@
     </row>
     <row r="14" spans="1:28">
       <c r="R14" s="4" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="S14" s="24" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="T14" s="27">
         <v>194</v>
@@ -4288,10 +4234,10 @@
     </row>
     <row r="15" spans="1:28">
       <c r="R15" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="T15" s="27">
         <v>78</v>
@@ -4472,10 +4418,10 @@
         <v>9</v>
       </c>
       <c r="AB3" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="AC3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:29">
@@ -4534,10 +4480,10 @@
         <v>9</v>
       </c>
       <c r="AB4" s="4" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="AC4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -4596,10 +4542,10 @@
         <v>9</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="AC5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -4649,10 +4595,10 @@
         <v>9</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="AC6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="31.5">
@@ -4702,10 +4648,10 @@
         <v>35</v>
       </c>
       <c r="AB7" s="25" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="AC7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="31.5">
@@ -4755,10 +4701,10 @@
         <v>35</v>
       </c>
       <c r="AB8" s="25" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="AC8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -4808,10 +4754,10 @@
         <v>45</v>
       </c>
       <c r="AB9" s="25" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="AC9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -4849,10 +4795,10 @@
         <v>45</v>
       </c>
       <c r="AB10" s="25" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="AC10" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -4890,10 +4836,10 @@
         <v>45</v>
       </c>
       <c r="AB11" s="25" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="AC11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="17.25" thickBot="1">
@@ -4931,26 +4877,26 @@
         <v>45</v>
       </c>
       <c r="AB12" s="25" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="AC12" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="17.25" thickTop="1">
       <c r="AB13" s="25" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="AC13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="AB14" s="25" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="AC14" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>